<commit_message>
update questionnaire and data extraction cards
</commit_message>
<xml_diff>
--- a/Literature mapping/stateoftheart_correct.xlsx
+++ b/Literature mapping/stateoftheart_correct.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Thesis2021\Literature mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F6AE49-6C93-4056-A890-2D43F52D3878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC8B9AF-28F7-42CE-A394-9949903BD845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6495" yWindow="-16410" windowWidth="14400" windowHeight="7365" tabRatio="917" firstSheet="11" activeTab="22" xr2:uid="{BEBBE7CD-C2EA-4C4E-939C-4EA0A7F78CED}"/>
+    <workbookView xWindow="-27195" yWindow="-20040" windowWidth="9600" windowHeight="6000" tabRatio="917" firstSheet="11" activeTab="22" xr2:uid="{BEBBE7CD-C2EA-4C4E-939C-4EA0A7F78CED}"/>
   </bookViews>
   <sheets>
     <sheet name="google Scholar" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">springerlink!$A$1:$B$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -68,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2784" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2760" uniqueCount="452">
   <si>
     <t>Search`</t>
   </si>
@@ -10737,7 +10736,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A77" sqref="A77"/>
+      <selection pane="bottomLeft" activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11629,44 +11628,20 @@
         <v>425</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>426</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>426</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>426</v>
-      </c>
-      <c r="H30" s="11" t="s">
-        <v>426</v>
-      </c>
-      <c r="I30" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="J30" s="11" t="s">
-        <v>426</v>
-      </c>
-      <c r="K30" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="L30" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="M30" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="N30" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="O30" s="12" t="s">
-        <v>70</v>
-      </c>
+        <v>431</v>
+      </c>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
     </row>
     <row r="31" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
@@ -11746,44 +11721,20 @@
         <v>425</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>426</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>426</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>426</v>
-      </c>
-      <c r="H33" s="11" t="s">
-        <v>426</v>
-      </c>
-      <c r="I33" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="J33" s="11" t="s">
-        <v>426</v>
-      </c>
-      <c r="K33" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="L33" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="M33" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="N33" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="O33" s="12" t="s">
-        <v>70</v>
-      </c>
+        <v>431</v>
+      </c>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
     </row>
     <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">

</xml_diff>